<commit_message>
exchange test case no. 49
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/split_payment_test_data.xlsx
+++ b/TestData/Web_POS/Billing/split_payment_test_data.xlsx
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>TC_20</t>
+  </si>
+  <si>
+    <t>cash : 275, store-credit : 275</t>
   </si>
   <si>
     <t>m3DOdg</t>
@@ -770,8 +773,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="O10">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="G10">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2893,7 +2896,7 @@
         <v>28</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>29</v>
@@ -2926,12 +2929,12 @@
         <v>32</v>
       </c>
       <c r="W21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" ht="32.25" customHeight="1">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
@@ -2964,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>29</v>
@@ -3002,7 +3005,7 @@
     </row>
     <row r="23" ht="28.5" customHeight="1">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>24</v>
@@ -3073,7 +3076,7 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>24</v>
@@ -3144,7 +3147,7 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>24</v>
@@ -3215,7 +3218,7 @@
     </row>
     <row r="26" ht="14.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>24</v>
@@ -3286,7 +3289,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>24</v>
@@ -3357,7 +3360,7 @@
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>24</v>
@@ -3411,7 +3414,7 @@
         <v>7709577438</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="T28" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Resolved errors of all sub modules of billing
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/split_payment_test_data.xlsx
+++ b/TestData/Web_POS/Billing/split_payment_test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Calc"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\PycharmProjects\zwing-qa-automation\TestData\Web_POS\Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Web_POS\Billing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>voucher_code</t>
+  </si>
+  <si>
+    <t>tax_invoice</t>
   </si>
   <si>
     <t>TC_1</t>
@@ -773,8 +776,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="G10">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="O24">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -866,22 +869,25 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>123456</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>123456</v>
@@ -893,66 +899,69 @@
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" s="4">
         <v>45384</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>123456</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>123456</v>
@@ -964,66 +973,69 @@
         <v>600</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O3" s="4">
         <v>45384</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="33" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7">
         <v>123456</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="7">
         <v>123456</v>
@@ -1035,10 +1047,10 @@
         <v>600</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
@@ -1047,54 +1059,57 @@
         <v>2</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O4" s="4">
         <v>45384</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="34.8" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="7">
         <v>123456</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7">
         <v>123456</v>
@@ -1106,10 +1121,10 @@
         <v>600</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -1118,54 +1133,57 @@
         <v>2</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O5" s="4">
         <v>45384</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="33.75" customHeight="1">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>123456</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3">
         <v>123456</v>
@@ -1177,7 +1195,7 @@
         <v>600</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -1186,57 +1204,60 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O6" s="4">
         <v>45384</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
         <v>123456</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3">
         <v>123456</v>
@@ -1248,7 +1269,7 @@
         <v>600</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J7" s="9">
         <v>1</v>
@@ -1257,57 +1278,60 @@
         <v>1</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O7" s="4">
         <v>45384</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R7" s="10">
         <v>7709577438</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="33.75" customHeight="1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>123456</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3">
         <v>123456</v>
@@ -1319,7 +1343,7 @@
         <v>600</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="9">
         <v>1</v>
@@ -1328,57 +1352,60 @@
         <v>1</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O8" s="4">
         <v>45384</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R8" s="10">
         <v>7709577438</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" ht="33.75" customHeight="1">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="7">
         <v>123456</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7">
         <v>123456</v>
@@ -1390,66 +1417,69 @@
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O9" s="4">
         <v>45384</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="33.75" customHeight="1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3">
         <v>123456</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7">
         <v>123456</v>
@@ -1461,66 +1491,69 @@
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O10" s="4">
         <v>45384</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3">
         <v>123456</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3">
         <v>123456</v>
@@ -1532,7 +1565,7 @@
         <v>600</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J11" s="9">
         <v>1</v>
@@ -1541,57 +1574,60 @@
         <v>1</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O11" s="4">
         <v>45384</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R11" s="10">
         <v>7709577438</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <v>123456</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3">
         <v>123456</v>
@@ -1603,7 +1639,7 @@
         <v>600</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -1612,57 +1648,60 @@
         <v>1</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O12" s="4">
         <v>45384</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R12" s="10">
         <v>7709577438</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3">
         <v>123456</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3">
         <v>123456</v>
@@ -1674,7 +1713,7 @@
         <v>600</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J13" s="9">
         <v>1</v>
@@ -1683,57 +1722,60 @@
         <v>1</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O13" s="4">
         <v>45384</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R13" s="10">
         <v>7709577438</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="26.25" customHeight="1">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3">
         <v>123456</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3">
         <v>123456</v>
@@ -1745,7 +1787,7 @@
         <v>600</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J14" s="9">
         <v>1</v>
@@ -1754,57 +1796,60 @@
         <v>1</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O14" s="4">
         <v>45384</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R14" s="10">
         <v>7709577438</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="11">
         <v>123456</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3">
         <v>123456</v>
@@ -1816,7 +1861,7 @@
         <v>600</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J15" s="9">
         <v>1</v>
@@ -1825,57 +1870,60 @@
         <v>1</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O15" s="4">
         <v>45384</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R15" s="10">
         <v>7709577438</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="14.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" s="7">
         <v>123456</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16" s="7">
         <v>123456</v>
@@ -1887,49 +1935,52 @@
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K16" s="1">
         <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O16" s="12">
         <v>45384</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
@@ -2579,19 +2630,19 @@
     </row>
     <row r="17" ht="31.5" customHeight="1">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3">
         <v>123456</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3">
         <v>123456</v>
@@ -2603,7 +2654,7 @@
         <v>600</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J17" s="9">
         <v>1</v>
@@ -2612,57 +2663,60 @@
         <v>1</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O17" s="4">
         <v>45384</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R17" s="10">
         <v>7709577438</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="31.5" customHeight="1">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="14">
         <v>123456</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18">
         <v>123456</v>
@@ -2674,66 +2728,69 @@
         <v>600</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O18" s="12">
         <v>45384</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7">
         <v>123456</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" s="7">
         <v>123456</v>
@@ -2745,10 +2802,10 @@
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K19" s="1">
         <v>1</v>
@@ -2757,54 +2814,57 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O19" s="12">
         <v>45384</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W19" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" ht="31.5" customHeight="1">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20">
         <v>123456</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>123456</v>
@@ -2816,66 +2876,69 @@
         <v>600</v>
       </c>
       <c r="I20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O20" s="12">
         <v>45384</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R20" s="10">
         <v>7709577438</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W20" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="31.5" customHeight="1">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <v>123456</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F21">
         <v>123456</v>
@@ -2887,66 +2950,69 @@
         <v>600</v>
       </c>
       <c r="I21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O21" s="12">
         <v>45384</v>
       </c>
       <c r="P21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R21" s="10">
         <v>7709577438</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T21" s="2">
         <v>300</v>
       </c>
       <c r="U21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W21" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" ht="32.25" customHeight="1">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="3">
         <v>123456</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3">
         <v>123456</v>
@@ -2958,7 +3024,7 @@
         <v>600</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J22" s="9">
         <v>1</v>
@@ -2967,57 +3033,60 @@
         <v>1</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O22" s="4">
         <v>45384</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R22" s="10">
         <v>7709577438</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" ht="28.5" customHeight="1">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3">
         <v>123456</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F23" s="3">
         <v>123456</v>
@@ -3029,7 +3098,7 @@
         <v>600</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J23" s="9">
         <v>1</v>
@@ -3038,57 +3107,60 @@
         <v>1</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O23" s="4">
         <v>45384</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R23" s="10">
         <v>7709577438</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W23" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3">
         <v>123456</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F24" s="3">
         <v>123456</v>
@@ -3100,7 +3172,7 @@
         <v>600</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J24" s="9">
         <v>1</v>
@@ -3109,57 +3181,60 @@
         <v>1</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O24" s="4">
         <v>45384</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R24" s="10">
         <v>7709577438</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" s="3">
         <v>123456</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F25" s="3">
         <v>123456</v>
@@ -3171,7 +3246,7 @@
         <v>600</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J25" s="9">
         <v>1</v>
@@ -3180,57 +3255,60 @@
         <v>1</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O25" s="4">
         <v>45384</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R25" s="10">
         <v>6375266109</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3">
         <v>123456</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F26" s="3">
         <v>123456</v>
@@ -3242,7 +3320,7 @@
         <v>600</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J26" s="9">
         <v>1</v>
@@ -3251,57 +3329,60 @@
         <v>1</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O26" s="4">
         <v>45384</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R26" s="10">
         <v>7709577438</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3">
         <v>123456</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F27" s="3">
         <v>123456</v>
@@ -3313,7 +3394,7 @@
         <v>600</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J27" s="9">
         <v>1</v>
@@ -3322,57 +3403,60 @@
         <v>1</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O27" s="4">
         <v>45384</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R27" s="10">
         <v>7709577438</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3">
         <v>123456</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F28" s="3">
         <v>123456</v>
@@ -3384,7 +3468,7 @@
         <v>600</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J28" s="9">
         <v>1</v>
@@ -3393,40 +3477,43 @@
         <v>1</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O28" s="4">
         <v>45384</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R28" s="10">
         <v>7709577438</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" ht="14.25">

</xml_diff>